<commit_message>
Names formatted and files merged properly
</commit_message>
<xml_diff>
--- a/Cleaned-Data/2015-Passouts/Sem-4_2015_Passout_cleaned.xlsx
+++ b/Cleaned-Data/2015-Passouts/Sem-4_2015_Passout_cleaned.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prashant/Downloads/Student-Placement-Guidance/Cleaned-Data/2015-Passouts/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="9180" yWindow="1460" windowWidth="16100" windowHeight="14980"/>
   </bookViews>
   <sheets>
     <sheet name="Sem-4_2015_Passout_cleaned" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1198,8 +1211,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1262,6 +1275,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1308,12 +1326,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1340,14 +1358,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1374,6 +1393,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1549,14 +1569,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="F190" sqref="F190"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="32.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:41">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1681,7 +1743,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>134201</v>
       </c>
@@ -1758,7 +1820,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>134202</v>
       </c>
@@ -1835,7 +1897,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>134203</v>
       </c>
@@ -1960,7 +2022,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>134204</v>
       </c>
@@ -2037,7 +2099,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>134205</v>
       </c>
@@ -2114,7 +2176,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>134206</v>
       </c>
@@ -2191,7 +2253,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>134207</v>
       </c>
@@ -2268,7 +2330,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>134208</v>
       </c>
@@ -2393,7 +2455,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>134209</v>
       </c>
@@ -2470,7 +2532,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>134210</v>
       </c>
@@ -2547,7 +2609,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:41">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>134211</v>
       </c>
@@ -2672,7 +2734,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>134212</v>
       </c>
@@ -2797,7 +2859,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>134213</v>
       </c>
@@ -2922,7 +2984,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>134214</v>
       </c>
@@ -3047,7 +3109,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>134215</v>
       </c>
@@ -3124,7 +3186,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:41">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>134216</v>
       </c>
@@ -3249,7 +3311,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:41">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>134217</v>
       </c>
@@ -3323,7 +3385,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="19" spans="1:41">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>134218</v>
       </c>
@@ -3448,7 +3510,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="1:41">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>134219</v>
       </c>
@@ -3573,7 +3635,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:41">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>134220</v>
       </c>
@@ -3650,7 +3712,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="22" spans="1:41">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>134221</v>
       </c>
@@ -3769,7 +3831,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="23" spans="1:41">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>134222</v>
       </c>
@@ -3894,7 +3956,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="24" spans="1:41">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>134223</v>
       </c>
@@ -4013,7 +4075,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:41">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>134224</v>
       </c>
@@ -4090,7 +4152,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="26" spans="1:41">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>134225</v>
       </c>
@@ -4164,7 +4226,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="1:41">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>134226</v>
       </c>
@@ -4289,7 +4351,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="28" spans="1:41">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>134227</v>
       </c>
@@ -4366,7 +4428,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="29" spans="1:41">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>134228</v>
       </c>
@@ -4491,7 +4553,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="30" spans="1:41">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>134229</v>
       </c>
@@ -4565,7 +4627,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="31" spans="1:41">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>134230</v>
       </c>
@@ -4642,7 +4704,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:41">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>134231</v>
       </c>
@@ -4716,7 +4778,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:41">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>134232</v>
       </c>
@@ -4793,7 +4855,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="34" spans="1:41">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>134233</v>
       </c>
@@ -4870,7 +4932,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="35" spans="1:41">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>134234</v>
       </c>
@@ -4983,7 +5045,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="36" spans="1:41">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>134235</v>
       </c>
@@ -5057,7 +5119,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="37" spans="1:41">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>134236</v>
       </c>
@@ -5134,7 +5196,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="38" spans="1:41">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>134237</v>
       </c>
@@ -5211,7 +5273,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="39" spans="1:41">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>134238</v>
       </c>
@@ -5288,7 +5350,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="40" spans="1:41">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>134239</v>
       </c>
@@ -5365,7 +5427,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="41" spans="1:41">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>134240</v>
       </c>
@@ -5442,7 +5504,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="42" spans="1:41">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>134241</v>
       </c>
@@ -5519,7 +5581,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="43" spans="1:41">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>134242</v>
       </c>
@@ -5596,7 +5658,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="44" spans="1:41">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>134243</v>
       </c>
@@ -5673,7 +5735,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="45" spans="1:41">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>134244</v>
       </c>
@@ -5798,7 +5860,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="46" spans="1:41">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>134245</v>
       </c>
@@ -5875,7 +5937,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="47" spans="1:41">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>134246</v>
       </c>
@@ -5952,7 +6014,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="48" spans="1:41">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>134247</v>
       </c>
@@ -6026,7 +6088,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="49" spans="1:41">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>134248</v>
       </c>
@@ -6151,7 +6213,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="50" spans="1:41">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>134249</v>
       </c>
@@ -6228,7 +6290,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="51" spans="1:41">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>134250</v>
       </c>
@@ -6305,7 +6367,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="52" spans="1:41">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>134251</v>
       </c>
@@ -6382,7 +6444,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="53" spans="1:41">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>134252</v>
       </c>
@@ -6459,7 +6521,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="54" spans="1:41">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>134253</v>
       </c>
@@ -6536,7 +6598,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="55" spans="1:41">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>134254</v>
       </c>
@@ -6613,7 +6675,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="56" spans="1:41">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>134255</v>
       </c>
@@ -6690,7 +6752,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="57" spans="1:41">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>134256</v>
       </c>
@@ -6767,7 +6829,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="58" spans="1:41">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>134257</v>
       </c>
@@ -6844,7 +6906,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="59" spans="1:41">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>134258</v>
       </c>
@@ -6969,7 +7031,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="60" spans="1:41">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>134259</v>
       </c>
@@ -7046,7 +7108,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="61" spans="1:41">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>134260</v>
       </c>
@@ -7171,7 +7233,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="62" spans="1:41">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>134261</v>
       </c>
@@ -7296,7 +7358,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="63" spans="1:41">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>134262</v>
       </c>
@@ -7370,7 +7432,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="64" spans="1:41">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>134263</v>
       </c>
@@ -7447,7 +7509,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="65" spans="1:41">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>134264</v>
       </c>
@@ -7572,7 +7634,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="66" spans="1:41">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>134265</v>
       </c>
@@ -7649,7 +7711,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="67" spans="1:41">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>134266</v>
       </c>
@@ -7726,7 +7788,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="68" spans="1:41">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>134267</v>
       </c>
@@ -7851,7 +7913,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="69" spans="1:41">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>134268</v>
       </c>
@@ -7976,7 +8038,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="70" spans="1:41">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>134269</v>
       </c>
@@ -8053,7 +8115,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="71" spans="1:41">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>134270</v>
       </c>
@@ -8130,7 +8192,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="72" spans="1:41">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>134271</v>
       </c>
@@ -8207,7 +8269,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="73" spans="1:41">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>134272</v>
       </c>
@@ -8284,7 +8346,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="74" spans="1:41">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>134273</v>
       </c>
@@ -8361,7 +8423,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="75" spans="1:41">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>134274</v>
       </c>
@@ -8486,7 +8548,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="76" spans="1:41">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>134275</v>
       </c>
@@ -8563,7 +8625,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="77" spans="1:41">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>134276</v>
       </c>
@@ -8640,7 +8702,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="78" spans="1:41">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>134277</v>
       </c>
@@ -8729,7 +8791,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="79" spans="1:41">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>134278</v>
       </c>
@@ -8854,7 +8916,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="80" spans="1:41">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>134279</v>
       </c>
@@ -8979,7 +9041,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="81" spans="1:41">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>134280</v>
       </c>
@@ -9104,7 +9166,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="82" spans="1:41">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>134281</v>
       </c>
@@ -9229,7 +9291,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="83" spans="1:41">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>134282</v>
       </c>
@@ -9354,7 +9416,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="84" spans="1:41">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>134283</v>
       </c>
@@ -9473,7 +9535,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="85" spans="1:41">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>134284</v>
       </c>
@@ -9550,7 +9612,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="86" spans="1:41">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>134285</v>
       </c>
@@ -9669,7 +9731,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="87" spans="1:41">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>134286</v>
       </c>
@@ -9794,7 +9856,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="88" spans="1:41">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>134287</v>
       </c>
@@ -9895,7 +9957,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="89" spans="1:41">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>134288</v>
       </c>
@@ -10020,7 +10082,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="90" spans="1:41">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>134289</v>
       </c>
@@ -10145,7 +10207,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="91" spans="1:41">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>134290</v>
       </c>
@@ -10270,7 +10332,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="92" spans="1:41">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>134291</v>
       </c>
@@ -10347,7 +10409,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="93" spans="1:41">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>134292</v>
       </c>
@@ -10472,7 +10534,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="94" spans="1:41">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>134293</v>
       </c>
@@ -10549,7 +10611,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="95" spans="1:41">
+    <row r="95" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>134294</v>
       </c>
@@ -10626,7 +10688,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="96" spans="1:41">
+    <row r="96" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>134295</v>
       </c>
@@ -10751,7 +10813,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="97" spans="1:41">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>134296</v>
       </c>
@@ -10828,7 +10890,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:41">
+    <row r="98" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>134297</v>
       </c>
@@ -10905,7 +10967,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="99" spans="1:41">
+    <row r="99" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>134298</v>
       </c>
@@ -10982,7 +11044,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="100" spans="1:41">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>134299</v>
       </c>
@@ -11059,7 +11121,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="101" spans="1:41">
+    <row r="101" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>134300</v>
       </c>
@@ -11184,7 +11246,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="102" spans="1:41">
+    <row r="102" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>134301</v>
       </c>
@@ -11309,7 +11371,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="103" spans="1:41">
+    <row r="103" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>134302</v>
       </c>
@@ -11434,7 +11496,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="104" spans="1:41">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>134303</v>
       </c>
@@ -11511,7 +11573,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="105" spans="1:41">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>134304</v>
       </c>
@@ -11588,7 +11650,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="106" spans="1:41">
+    <row r="106" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>134305</v>
       </c>
@@ -11713,7 +11775,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="107" spans="1:41">
+    <row r="107" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>134306</v>
       </c>
@@ -11838,7 +11900,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="108" spans="1:41">
+    <row r="108" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>134307</v>
       </c>
@@ -11915,7 +11977,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="109" spans="1:41">
+    <row r="109" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>134308</v>
       </c>
@@ -11992,7 +12054,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="110" spans="1:41">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>134309</v>
       </c>
@@ -12069,7 +12131,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="111" spans="1:41">
+    <row r="111" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>134310</v>
       </c>
@@ -12146,7 +12208,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="112" spans="1:41">
+    <row r="112" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>134311</v>
       </c>
@@ -12223,7 +12285,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="113" spans="1:41">
+    <row r="113" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>134312</v>
       </c>
@@ -12300,7 +12362,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="114" spans="1:41">
+    <row r="114" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>134313</v>
       </c>
@@ -12377,7 +12439,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="115" spans="1:41">
+    <row r="115" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>134314</v>
       </c>
@@ -12454,7 +12516,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="116" spans="1:41">
+    <row r="116" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>134315</v>
       </c>
@@ -12531,7 +12593,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="117" spans="1:41">
+    <row r="117" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>134316</v>
       </c>
@@ -12656,7 +12718,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="118" spans="1:41">
+    <row r="118" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>134317</v>
       </c>
@@ -12733,7 +12795,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="119" spans="1:41">
+    <row r="119" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>134318</v>
       </c>
@@ -12858,7 +12920,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="120" spans="1:41">
+    <row r="120" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>134319</v>
       </c>
@@ -12935,7 +12997,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="121" spans="1:41">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>134320</v>
       </c>
@@ -13054,7 +13116,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="122" spans="1:41">
+    <row r="122" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>134321</v>
       </c>
@@ -13131,7 +13193,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="123" spans="1:41">
+    <row r="123" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>134322</v>
       </c>
@@ -13208,7 +13270,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="124" spans="1:41">
+    <row r="124" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>134323</v>
       </c>
@@ -13285,7 +13347,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="125" spans="1:41">
+    <row r="125" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>134324</v>
       </c>
@@ -13362,7 +13424,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="126" spans="1:41">
+    <row r="126" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>134325</v>
       </c>
@@ -13487,7 +13549,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="127" spans="1:41">
+    <row r="127" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>134326</v>
       </c>
@@ -13564,7 +13626,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="128" spans="1:41">
+    <row r="128" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>134327</v>
       </c>
@@ -13641,7 +13703,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="129" spans="1:41">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>134328</v>
       </c>
@@ -13718,7 +13780,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="130" spans="1:41">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>134329</v>
       </c>
@@ -13795,7 +13857,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="131" spans="1:41">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>134330</v>
       </c>
@@ -13872,7 +13934,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="132" spans="1:41">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>134331</v>
       </c>
@@ -13997,7 +14059,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="133" spans="1:41">
+    <row r="133" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>134332</v>
       </c>
@@ -14074,7 +14136,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="134" spans="1:41">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>134333</v>
       </c>
@@ -14151,7 +14213,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="135" spans="1:41">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>134334</v>
       </c>
@@ -14270,7 +14332,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="136" spans="1:41">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134335</v>
       </c>
@@ -14395,7 +14457,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="137" spans="1:41">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>134336</v>
       </c>
@@ -14520,7 +14582,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="138" spans="1:41">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>134337</v>
       </c>
@@ -14597,7 +14659,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="139" spans="1:41">
+    <row r="139" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>134338</v>
       </c>
@@ -14722,7 +14784,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="140" spans="1:41">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>134339</v>
       </c>
@@ -14847,7 +14909,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="141" spans="1:41">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>134340</v>
       </c>
@@ -14972,7 +15034,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="142" spans="1:41">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>134341</v>
       </c>
@@ -15049,7 +15111,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="143" spans="1:41">
+    <row r="143" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>134342</v>
       </c>
@@ -15126,7 +15188,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="144" spans="1:41">
+    <row r="144" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>134343</v>
       </c>
@@ -15251,7 +15313,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="145" spans="1:41">
+    <row r="145" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>134344</v>
       </c>
@@ -15346,7 +15408,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="146" spans="1:41">
+    <row r="146" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>134345</v>
       </c>
@@ -15471,7 +15533,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="147" spans="1:41">
+    <row r="147" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>134346</v>
       </c>
@@ -15596,7 +15658,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="148" spans="1:41">
+    <row r="148" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>134347</v>
       </c>
@@ -15721,7 +15783,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="149" spans="1:41">
+    <row r="149" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>134348</v>
       </c>
@@ -15846,7 +15908,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="150" spans="1:41">
+    <row r="150" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>134349</v>
       </c>
@@ -15953,7 +16015,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="151" spans="1:41">
+    <row r="151" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>134350</v>
       </c>
@@ -16075,7 +16137,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="152" spans="1:41">
+    <row r="152" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>134351</v>
       </c>
@@ -16194,7 +16256,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="153" spans="1:41">
+    <row r="153" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>134352</v>
       </c>
@@ -16316,7 +16378,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="154" spans="1:41">
+    <row r="154" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>134353</v>
       </c>
@@ -16441,7 +16503,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="155" spans="1:41">
+    <row r="155" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>134354</v>
       </c>
@@ -16566,7 +16628,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="156" spans="1:41">
+    <row r="156" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>134355</v>
       </c>
@@ -16688,7 +16750,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="157" spans="1:41">
+    <row r="157" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>134356</v>
       </c>
@@ -16813,7 +16875,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="158" spans="1:41">
+    <row r="158" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>134357</v>
       </c>
@@ -16935,7 +16997,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="159" spans="1:41">
+    <row r="159" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>134358</v>
       </c>
@@ -17057,7 +17119,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="160" spans="1:41">
+    <row r="160" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>134359</v>
       </c>
@@ -17182,7 +17244,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="161" spans="1:41">
+    <row r="161" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>134360</v>
       </c>
@@ -17283,7 +17345,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="162" spans="1:41">
+    <row r="162" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>134361</v>
       </c>
@@ -17408,7 +17470,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="163" spans="1:41">
+    <row r="163" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>134362</v>
       </c>
@@ -17527,7 +17589,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="164" spans="1:41">
+    <row r="164" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>134363</v>
       </c>
@@ -17652,7 +17714,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="165" spans="1:41">
+    <row r="165" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>134364</v>
       </c>
@@ -17774,7 +17836,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="166" spans="1:41">
+    <row r="166" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>134365</v>
       </c>
@@ -17890,7 +17952,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="167" spans="1:41">
+    <row r="167" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>134366</v>
       </c>
@@ -18012,7 +18074,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="168" spans="1:41">
+    <row r="168" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>134367</v>
       </c>
@@ -18137,7 +18199,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="169" spans="1:41">
+    <row r="169" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>134368</v>
       </c>
@@ -18259,7 +18321,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="170" spans="1:41">
+    <row r="170" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>134369</v>
       </c>
@@ -18384,7 +18446,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="171" spans="1:41">
+    <row r="171" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>134370</v>
       </c>
@@ -18506,7 +18568,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="172" spans="1:41">
+    <row r="172" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>134371</v>
       </c>
@@ -18628,7 +18690,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="173" spans="1:41">
+    <row r="173" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>134372</v>
       </c>
@@ -18753,7 +18815,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="174" spans="1:41">
+    <row r="174" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>134373</v>
       </c>
@@ -18875,7 +18937,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="175" spans="1:41">
+    <row r="175" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>134374</v>
       </c>
@@ -18994,7 +19056,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="176" spans="1:41">
+    <row r="176" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>134375</v>
       </c>
@@ -19116,7 +19178,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="177" spans="1:41">
+    <row r="177" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>134376</v>
       </c>
@@ -19241,7 +19303,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="178" spans="1:41">
+    <row r="178" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>134377</v>
       </c>
@@ -19342,7 +19404,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="179" spans="1:41">
+    <row r="179" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>134378</v>
       </c>
@@ -19461,7 +19523,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="180" spans="1:41">
+    <row r="180" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>134379</v>
       </c>
@@ -19586,7 +19648,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="181" spans="1:41">
+    <row r="181" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>134380</v>
       </c>
@@ -19711,7 +19773,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="182" spans="1:41">
+    <row r="182" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>134381</v>
       </c>
@@ -19836,7 +19898,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="183" spans="1:41">
+    <row r="183" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>134382</v>
       </c>

</xml_diff>